<commit_message>
Manually add some gene family annotations to hmm profile name in Yutin Excel file. In Excel file manually curated names marked in blue.
</commit_message>
<xml_diff>
--- a/input_files/Yutin conserved genes 41564_2017_53_MOESM3_ESM.xlsx
+++ b/input_files/Yutin conserved genes 41564_2017_53_MOESM3_ESM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\17 Dutihl Lab\crassphage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\17 Dutihl Lab\source\phages_pycharm\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="487">
   <si>
     <t>crAssphage_JQ995537</t>
   </si>
@@ -530,9 +530,6 @@
     <t xml:space="preserve"> -</t>
   </si>
   <si>
-    <t>b-b’ RNAP</t>
-  </si>
-  <si>
     <t>46N</t>
   </si>
   <si>
@@ -581,13 +578,7 @@
     <t>gene23</t>
   </si>
   <si>
-    <t xml:space="preserve">ssb </t>
-  </si>
-  <si>
     <t>gene21</t>
-  </si>
-  <si>
-    <t>RecT</t>
   </si>
   <si>
     <t>gene19</t>
@@ -1524,12 +1515,51 @@
   <si>
     <t>alternative names used in Supplementary_Note_1</t>
   </si>
+  <si>
+    <t>ligase25</t>
+  </si>
+  <si>
+    <t>Ligase</t>
+  </si>
+  <si>
+    <t>Uracil-DNA glycosylase</t>
+  </si>
+  <si>
+    <t>Major Capsid Protein</t>
+  </si>
+  <si>
+    <t>single stranded DNA-binding pr.</t>
+  </si>
+  <si>
+    <t>Polymerase A</t>
+  </si>
+  <si>
+    <t>Polymerase B</t>
+  </si>
+  <si>
+    <t>ThyX</t>
+  </si>
+  <si>
+    <t>Flavin-dependent thymidylate synthase</t>
+  </si>
+  <si>
+    <t>phage RecT recombinase</t>
+  </si>
+  <si>
+    <t>dUTP</t>
+  </si>
+  <si>
+    <t>dUTP diphosphatase</t>
+  </si>
+  <si>
+    <t>b-b-prime RNAP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1740,6 +1770,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1782,7 +1819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2029,6 +2066,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2387,7 +2425,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="10"/>
@@ -3533,9 +3571,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X38"/>
+  <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -3547,16 +3587,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="E1" s="104" t="s">
+      <c r="E1" s="105" t="s">
         <v>123</v>
       </c>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
-      <c r="N1" s="105" t="s">
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="N1" s="106" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="105" t="s">
+      <c r="V1" s="106" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3600,7 +3640,7 @@
       <c r="M2" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="106"/>
+      <c r="N2" s="107"/>
       <c r="O2" s="55" t="s">
         <v>21</v>
       </c>
@@ -3622,7 +3662,7 @@
       <c r="U2" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="V2" s="106"/>
+      <c r="V2" s="107"/>
       <c r="W2" s="55" t="s">
         <v>38</v>
       </c>
@@ -3905,8 +3945,8 @@
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A7" s="15" t="s">
-        <v>137</v>
+      <c r="A7" s="104" t="s">
+        <v>477</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>137</v>
@@ -4502,14 +4542,14 @@
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A16" s="59" t="s">
-        <v>153</v>
+      <c r="A16" s="104" t="s">
+        <v>486</v>
       </c>
       <c r="B16" s="59" t="s">
         <v>152</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D16" s="13">
         <v>49</v>
@@ -4580,7 +4620,7 @@
         <v>152</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D17" s="13">
         <v>48</v>
@@ -4598,16 +4638,16 @@
         <v>130</v>
       </c>
       <c r="I17" s="52" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J17" s="53" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K17" s="53" t="s">
         <v>130</v>
       </c>
       <c r="L17" s="53" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M17" s="53" t="s">
         <v>130</v>
@@ -4645,16 +4685,16 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A18" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>157</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>158</v>
       </c>
       <c r="C18" s="13">
         <v>22</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E18" s="62" t="s">
         <v>130</v>
@@ -4704,10 +4744,10 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A19" s="15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C19" s="13">
         <v>18</v>
@@ -4754,10 +4794,10 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A20" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>162</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>163</v>
       </c>
       <c r="C20" s="13">
         <v>86</v>
@@ -4810,10 +4850,10 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A21" s="59" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B21" s="59" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C21" s="13">
         <v>49</v>
@@ -4825,7 +4865,7 @@
         <v>130</v>
       </c>
       <c r="F21" s="62" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G21" s="62" t="s">
         <v>130</v>
@@ -4862,10 +4902,10 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A22" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C22" s="13">
         <v>34</v>
@@ -4897,10 +4937,10 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A23" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B23" s="15" t="s">
         <v>167</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>168</v>
       </c>
       <c r="C23" s="13">
         <v>32</v>
@@ -4926,10 +4966,10 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A24" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C24" s="13">
         <v>23</v>
@@ -4951,11 +4991,11 @@
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A25" s="15" t="s">
-        <v>170</v>
+      <c r="A25" s="104" t="s">
+        <v>478</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C25" s="13">
         <v>21</v>
@@ -4977,11 +5017,11 @@
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A26" s="15" t="s">
-        <v>172</v>
+      <c r="A26" s="104" t="s">
+        <v>483</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C26" s="13">
         <v>19</v>
@@ -5003,11 +5043,11 @@
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A27" s="15" t="s">
-        <v>174</v>
+      <c r="A27" s="104" t="s">
+        <v>480</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C27" s="13">
         <v>17</v>
@@ -5042,10 +5082,10 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A28" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C28" s="13">
         <v>20</v>
@@ -5067,11 +5107,11 @@
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A29" s="15" t="s">
-        <v>176</v>
+      <c r="A29" s="104" t="s">
+        <v>476</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C29" s="13">
         <v>16</v>
@@ -5115,10 +5155,10 @@
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A30" s="15" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C30" s="13">
         <v>15</v>
@@ -5141,10 +5181,10 @@
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A31" s="15" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>152</v>
@@ -5176,10 +5216,10 @@
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A32" s="15" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>152</v>
@@ -5229,10 +5269,10 @@
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A33" s="15" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>152</v>
@@ -5279,10 +5319,10 @@
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A34" s="15" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>152</v>
@@ -5308,10 +5348,10 @@
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A35" s="15" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>152</v>
@@ -5340,10 +5380,10 @@
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A36" s="59" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B36" s="59" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>152</v>
@@ -5369,10 +5409,10 @@
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A37" s="59" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B37" s="59" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>152</v>
@@ -5397,11 +5437,11 @@
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A38" s="15" t="s">
-        <v>190</v>
+      <c r="A38" s="104" t="s">
+        <v>479</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>152</v>
@@ -5426,6 +5466,30 @@
       </c>
       <c r="W38" s="53" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A39" s="104" t="s">
+        <v>475</v>
+      </c>
+      <c r="B39" s="104" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A40" s="104" t="s">
+        <v>482</v>
+      </c>
+      <c r="B40" s="104" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A41" s="104" t="s">
+        <v>485</v>
+      </c>
+      <c r="B41" s="104" t="s">
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -5435,6 +5499,7 @@
     <mergeCell ref="V1:V2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5442,9 +5507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T493"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A373" sqref="A373"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -5470,7 +5533,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="F1" s="46"/>
       <c r="G1" s="46"/>
@@ -5488,7 +5551,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="F2" s="46"/>
       <c r="G2" s="46"/>
@@ -5506,7 +5569,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="F3" s="46"/>
       <c r="G3" s="46"/>
@@ -5524,7 +5587,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="F4" s="46"/>
       <c r="G4" s="46"/>
@@ -5542,7 +5605,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="E5" s="96"/>
       <c r="F5" s="46"/>
@@ -5561,7 +5624,7 @@
     </row>
     <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="E6" s="96"/>
       <c r="F6" s="46"/>
@@ -5580,7 +5643,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="E7" s="96"/>
       <c r="F7" s="46"/>
@@ -5599,7 +5662,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="E8" s="96"/>
       <c r="F8" s="46"/>
@@ -5618,7 +5681,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="E9" s="96"/>
       <c r="F9" s="46"/>
@@ -5653,69 +5716,69 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.45">
       <c r="C11" s="63" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="43"/>
       <c r="F11" s="3"/>
       <c r="G11" s="64"/>
       <c r="H11" s="65" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I11" s="66"/>
       <c r="J11" s="67"/>
       <c r="K11" s="66"/>
       <c r="L11" s="68"/>
       <c r="M11" s="65" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="N11" s="69"/>
       <c r="O11" s="70"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" s="74" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="E12" s="43" t="s">
         <v>196</v>
       </c>
-      <c r="C12" s="74" t="s">
+      <c r="F12" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="E12" s="43" t="s">
-        <v>199</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="G12" s="64"/>
       <c r="H12" s="74" t="s">
+        <v>194</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="J12" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="J12" s="43" t="s">
-        <v>199</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="L12" s="64"/>
       <c r="M12" s="74" t="s">
+        <v>194</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="O12" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="P12" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="O12" s="43" t="s">
-        <v>199</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="Q12" s="75"/>
     </row>
@@ -5747,7 +5810,7 @@
         <v>110</v>
       </c>
       <c r="B14" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C14" s="86">
         <v>35.380000000000003</v>
@@ -5779,7 +5842,7 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C15" s="86">
         <v>31.518999999999998</v>
@@ -5811,7 +5874,7 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C16" s="86">
         <v>35.119</v>
@@ -5843,7 +5906,7 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C17" s="86">
         <v>31.503</v>
@@ -5875,7 +5938,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C18" s="86">
         <v>23.292000000000002</v>
@@ -5917,7 +5980,7 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C21" s="86">
         <v>25.478999999999999</v>
@@ -5937,7 +6000,7 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C22" s="86">
         <v>25.835999999999999</v>
@@ -5969,7 +6032,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C23" s="86">
         <v>23.033999999999999</v>
@@ -5989,7 +6052,7 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C24" s="86">
         <v>21.829000000000001</v>
@@ -6019,7 +6082,7 @@
         <v>111</v>
       </c>
       <c r="B27" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C27" s="86">
         <v>24.1</v>
@@ -6051,7 +6114,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C28" s="86">
         <v>26.734999999999999</v>
@@ -6083,7 +6146,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C29" s="86">
         <v>27.193000000000001</v>
@@ -6115,7 +6178,7 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C30" s="86">
         <v>29.885000000000002</v>
@@ -6159,7 +6222,7 @@
         <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C31" s="86">
         <v>22.315999999999999</v>
@@ -6191,7 +6254,7 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C32" s="86">
         <v>26.210999999999999</v>
@@ -6246,7 +6309,7 @@
         <v>110</v>
       </c>
       <c r="B34" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C34" s="86">
         <v>35.177</v>
@@ -6291,7 +6354,7 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C35" s="86">
         <v>32.584000000000003</v>
@@ -6336,7 +6399,7 @@
         <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C36" s="86">
         <v>32.28</v>
@@ -6381,7 +6444,7 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C37" s="86">
         <v>31.66</v>
@@ -6426,7 +6489,7 @@
         <v>14</v>
       </c>
       <c r="B38" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C38" s="86">
         <v>37.621000000000002</v>
@@ -6471,7 +6534,7 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C39" s="86">
         <v>53.636000000000003</v>
@@ -6516,7 +6579,7 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C40" s="86">
         <v>54.198</v>
@@ -6561,7 +6624,7 @@
         <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C41" s="86">
         <v>45.137999999999998</v>
@@ -6606,7 +6669,7 @@
         <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C42" s="86">
         <v>45.95</v>
@@ -6651,7 +6714,7 @@
         <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C43" s="86">
         <v>46.277000000000001</v>
@@ -6696,7 +6759,7 @@
         <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C44" s="86">
         <v>31.164999999999999</v>
@@ -6741,7 +6804,7 @@
         <v>23</v>
       </c>
       <c r="B45" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C45" s="86">
         <v>34.691000000000003</v>
@@ -6774,7 +6837,7 @@
         <v>24</v>
       </c>
       <c r="B46" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C46" s="86">
         <v>25.986000000000001</v>
@@ -6819,7 +6882,7 @@
         <v>111</v>
       </c>
       <c r="B47" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C47" s="86">
         <v>30.614999999999998</v>
@@ -6864,7 +6927,7 @@
         <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C48" s="86">
         <v>40.331000000000003</v>
@@ -6909,7 +6972,7 @@
         <v>30</v>
       </c>
       <c r="B49" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C49" s="86">
         <v>46.417999999999999</v>
@@ -6954,7 +7017,7 @@
         <v>31</v>
       </c>
       <c r="B50" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C50" s="86">
         <v>35.713999999999999</v>
@@ -6999,7 +7062,7 @@
         <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C51" s="86">
         <v>34.280999999999999</v>
@@ -7044,7 +7107,7 @@
         <v>38</v>
       </c>
       <c r="B52" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C52" s="86">
         <v>38.671999999999997</v>
@@ -7112,7 +7175,7 @@
         <v>110</v>
       </c>
       <c r="B54" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C54" s="86">
         <v>32.475000000000001</v>
@@ -7156,7 +7219,7 @@
         <v>5</v>
       </c>
       <c r="B55" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C55" s="86">
         <v>29.529</v>
@@ -7200,7 +7263,7 @@
         <v>6</v>
       </c>
       <c r="B56" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C56" s="86">
         <v>30.73</v>
@@ -7244,7 +7307,7 @@
         <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C57" s="86">
         <v>30.741</v>
@@ -7288,7 +7351,7 @@
         <v>14</v>
       </c>
       <c r="B58" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C58" s="86">
         <v>30.864000000000001</v>
@@ -7332,7 +7395,7 @@
         <v>7</v>
       </c>
       <c r="B59" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C59" s="86">
         <v>41.89</v>
@@ -7376,7 +7439,7 @@
         <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C60" s="86">
         <v>43.204999999999998</v>
@@ -7420,7 +7483,7 @@
         <v>17</v>
       </c>
       <c r="B61" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C61" s="86">
         <v>36.024999999999999</v>
@@ -7464,7 +7527,7 @@
         <v>19</v>
       </c>
       <c r="B62" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C62" s="86">
         <v>36.161999999999999</v>
@@ -7508,7 +7571,7 @@
         <v>20</v>
       </c>
       <c r="B63" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C63" s="86">
         <v>41.689</v>
@@ -7552,7 +7615,7 @@
         <v>21</v>
       </c>
       <c r="B64" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C64" s="86">
         <v>30.797999999999998</v>
@@ -7596,7 +7659,7 @@
         <v>23</v>
       </c>
       <c r="B65" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C65" s="86">
         <v>34.131</v>
@@ -7640,7 +7703,7 @@
         <v>24</v>
       </c>
       <c r="B66" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C66" s="86">
         <v>24.027000000000001</v>
@@ -7684,7 +7747,7 @@
         <v>111</v>
       </c>
       <c r="B67" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C67" s="86">
         <v>29.384</v>
@@ -7728,7 +7791,7 @@
         <v>29</v>
       </c>
       <c r="B68" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C68" s="86">
         <v>35.749000000000002</v>
@@ -7772,7 +7835,7 @@
         <v>30</v>
       </c>
       <c r="B69" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C69" s="86">
         <v>45.244</v>
@@ -7816,7 +7879,7 @@
         <v>31</v>
       </c>
       <c r="B70" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C70" s="86">
         <v>41.895000000000003</v>
@@ -7860,7 +7923,7 @@
         <v>37</v>
       </c>
       <c r="B71" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C71" s="86">
         <v>36.914000000000001</v>
@@ -7904,7 +7967,7 @@
         <v>38</v>
       </c>
       <c r="B72" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C72" s="86">
         <v>36.654000000000003</v>
@@ -7971,7 +8034,7 @@
         <v>110</v>
       </c>
       <c r="B74" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C74" s="86">
         <v>27.027000000000001</v>
@@ -8003,7 +8066,7 @@
         <v>5</v>
       </c>
       <c r="B75" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C75" s="86">
         <v>24.667999999999999</v>
@@ -8035,7 +8098,7 @@
         <v>6</v>
       </c>
       <c r="B76" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C76" s="86">
         <v>24.298999999999999</v>
@@ -8079,7 +8142,7 @@
         <v>4</v>
       </c>
       <c r="B77" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C77" s="86">
         <v>16.850999999999999</v>
@@ -8099,7 +8162,7 @@
         <v>14</v>
       </c>
       <c r="B78" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C78" s="86">
         <v>26.05</v>
@@ -8131,7 +8194,7 @@
         <v>7</v>
       </c>
       <c r="B79" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C79" s="86">
         <v>40.826999999999998</v>
@@ -8163,7 +8226,7 @@
         <v>10</v>
       </c>
       <c r="B80" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C80" s="86">
         <v>39.637</v>
@@ -8195,7 +8258,7 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C81" s="86">
         <v>27.568999999999999</v>
@@ -8215,7 +8278,7 @@
         <v>19</v>
       </c>
       <c r="B82" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C82" s="86">
         <v>24.332000000000001</v>
@@ -8235,7 +8298,7 @@
         <v>20</v>
       </c>
       <c r="B83" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C83" s="86">
         <v>26.815999999999999</v>
@@ -8255,7 +8318,7 @@
         <v>21</v>
       </c>
       <c r="B84" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C84" s="86">
         <v>16.446000000000002</v>
@@ -8280,7 +8343,7 @@
         <v>24</v>
       </c>
       <c r="B86" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C86" s="86">
         <v>15.680999999999999</v>
@@ -8300,7 +8363,7 @@
         <v>111</v>
       </c>
       <c r="B87" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C87" s="86">
         <v>18.228000000000002</v>
@@ -8320,7 +8383,7 @@
         <v>29</v>
       </c>
       <c r="B88" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C88" s="86">
         <v>24.478999999999999</v>
@@ -8352,7 +8415,7 @@
         <v>30</v>
       </c>
       <c r="B89" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C89" s="86">
         <v>31.670999999999999</v>
@@ -8384,7 +8447,7 @@
         <v>31</v>
       </c>
       <c r="B90" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C90" s="86">
         <v>32.021000000000001</v>
@@ -8404,7 +8467,7 @@
         <v>37</v>
       </c>
       <c r="B91" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C91" s="86">
         <v>24.119</v>
@@ -8436,7 +8499,7 @@
         <v>38</v>
       </c>
       <c r="B92" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C92" s="86">
         <v>24.4</v>
@@ -8491,7 +8554,7 @@
         <v>110</v>
       </c>
       <c r="B94" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C94" s="86">
         <v>37.677999999999997</v>
@@ -8523,7 +8586,7 @@
         <v>5</v>
       </c>
       <c r="B95" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C95" s="86">
         <v>35.281999999999996</v>
@@ -8567,7 +8630,7 @@
         <v>6</v>
       </c>
       <c r="B96" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C96" s="86">
         <v>35.091000000000001</v>
@@ -8599,7 +8662,7 @@
         <v>4</v>
       </c>
       <c r="B97" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C97" s="86">
         <v>36.585000000000001</v>
@@ -8631,7 +8694,7 @@
         <v>14</v>
       </c>
       <c r="B98" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C98" s="86">
         <v>32.033000000000001</v>
@@ -8675,7 +8738,7 @@
         <v>7</v>
       </c>
       <c r="B99" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C99" s="86">
         <v>47.726999999999997</v>
@@ -8707,7 +8770,7 @@
         <v>10</v>
       </c>
       <c r="B100" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C100" s="86">
         <v>48.148000000000003</v>
@@ -8751,7 +8814,7 @@
         <v>17</v>
       </c>
       <c r="B101" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C101" s="86">
         <v>40.963999999999999</v>
@@ -8795,7 +8858,7 @@
         <v>19</v>
       </c>
       <c r="B102" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C102" s="86">
         <v>38.854999999999997</v>
@@ -8839,7 +8902,7 @@
         <v>20</v>
       </c>
       <c r="B103" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C103" s="86">
         <v>38.618000000000002</v>
@@ -8883,7 +8946,7 @@
         <v>21</v>
       </c>
       <c r="B104" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C104" s="86">
         <v>32.277999999999999</v>
@@ -8927,7 +8990,7 @@
         <v>23</v>
       </c>
       <c r="B105" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C105" s="86">
         <v>29.643999999999998</v>
@@ -8959,7 +9022,7 @@
         <v>24</v>
       </c>
       <c r="B106" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C106" s="86">
         <v>22.8</v>
@@ -9003,7 +9066,7 @@
         <v>111</v>
       </c>
       <c r="B107" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C107" s="86">
         <v>24.047999999999998</v>
@@ -9023,7 +9086,7 @@
         <v>29</v>
       </c>
       <c r="B108" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C108" s="86">
         <v>36.863999999999997</v>
@@ -9067,7 +9130,7 @@
         <v>30</v>
       </c>
       <c r="B109" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C109" s="86">
         <v>45.061999999999998</v>
@@ -9111,7 +9174,7 @@
         <v>31</v>
       </c>
       <c r="B110" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C110" s="86">
         <v>39.712000000000003</v>
@@ -9155,7 +9218,7 @@
         <v>37</v>
       </c>
       <c r="B111" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C111" s="86">
         <v>30.664000000000001</v>
@@ -9187,7 +9250,7 @@
         <v>38</v>
       </c>
       <c r="B112" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C112" s="86">
         <v>28.88</v>
@@ -9216,7 +9279,7 @@
     </row>
     <row r="113" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A113" s="76" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C113" s="78"/>
       <c r="D113" s="75"/>
@@ -9242,7 +9305,7 @@
         <v>110</v>
       </c>
       <c r="B114" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C114" s="86">
         <v>25.518999999999998</v>
@@ -9274,7 +9337,7 @@
         <v>5</v>
       </c>
       <c r="B115" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C115" s="86">
         <v>25.683</v>
@@ -9306,7 +9369,7 @@
         <v>6</v>
       </c>
       <c r="B116" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C116" s="86">
         <v>27.245999999999999</v>
@@ -9338,7 +9401,7 @@
         <v>4</v>
       </c>
       <c r="B117" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C117" s="86">
         <v>31.183</v>
@@ -9370,7 +9433,7 @@
         <v>14</v>
       </c>
       <c r="B118" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C118" s="86">
         <v>25.552</v>
@@ -9414,7 +9477,7 @@
         <v>7</v>
       </c>
       <c r="B119" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C119" s="86">
         <v>42.646999999999998</v>
@@ -9458,7 +9521,7 @@
         <v>10</v>
       </c>
       <c r="B120" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C120" s="86">
         <v>43.015000000000001</v>
@@ -9502,7 +9565,7 @@
         <v>17</v>
       </c>
       <c r="B121" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C121" s="86">
         <v>35.686</v>
@@ -9522,7 +9585,7 @@
         <v>19</v>
       </c>
       <c r="B122" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C122" s="86">
         <v>32.584000000000003</v>
@@ -9554,7 +9617,7 @@
         <v>20</v>
       </c>
       <c r="B123" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C123" s="86">
         <v>33.076999999999998</v>
@@ -9586,7 +9649,7 @@
         <v>21</v>
       </c>
       <c r="B124" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C124" s="86">
         <v>18.146999999999998</v>
@@ -9606,7 +9669,7 @@
         <v>23</v>
       </c>
       <c r="B125" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C125" s="86">
         <v>25</v>
@@ -9638,7 +9701,7 @@
         <v>24</v>
       </c>
       <c r="B126" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C126" s="86">
         <v>23.466000000000001</v>
@@ -9658,7 +9721,7 @@
         <v>111</v>
       </c>
       <c r="B127" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C127" s="86">
         <v>23.462</v>
@@ -9678,7 +9741,7 @@
         <v>29</v>
       </c>
       <c r="B128" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C128" s="86">
         <v>27.306000000000001</v>
@@ -9710,7 +9773,7 @@
         <v>30</v>
       </c>
       <c r="B129" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C129" s="86">
         <v>33.729999999999997</v>
@@ -9754,7 +9817,7 @@
         <v>31</v>
       </c>
       <c r="B130" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C130" s="86">
         <v>32.341999999999999</v>
@@ -9798,7 +9861,7 @@
         <v>37</v>
       </c>
       <c r="B131" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C131" s="86">
         <v>27.757999999999999</v>
@@ -9830,7 +9893,7 @@
         <v>38</v>
       </c>
       <c r="B132" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C132" s="86">
         <v>28.268999999999998</v>
@@ -9859,7 +9922,7 @@
     </row>
     <row r="133" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A133" s="76" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C133" s="78"/>
       <c r="D133" s="75"/>
@@ -9885,7 +9948,7 @@
         <v>110</v>
       </c>
       <c r="B134" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C134" s="86">
         <v>35.128</v>
@@ -9929,7 +9992,7 @@
         <v>5</v>
       </c>
       <c r="B135" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C135" s="86">
         <v>32.506999999999998</v>
@@ -9973,7 +10036,7 @@
         <v>6</v>
       </c>
       <c r="B136" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C136" s="86">
         <v>36.517000000000003</v>
@@ -10017,7 +10080,7 @@
         <v>4</v>
       </c>
       <c r="B137" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C137" s="86">
         <v>33.710999999999999</v>
@@ -10061,7 +10124,7 @@
         <v>14</v>
       </c>
       <c r="B138" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C138" s="86">
         <v>33.634</v>
@@ -10105,7 +10168,7 @@
         <v>7</v>
       </c>
       <c r="B139" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C139" s="86">
         <v>44.048000000000002</v>
@@ -10149,7 +10212,7 @@
         <v>10</v>
       </c>
       <c r="B140" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C140" s="86">
         <v>45.536000000000001</v>
@@ -10193,7 +10256,7 @@
         <v>17</v>
       </c>
       <c r="B141" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C141" s="86">
         <v>35.244</v>
@@ -10242,7 +10305,7 @@
         <v>20</v>
       </c>
       <c r="B143" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C143" s="86">
         <v>38.154000000000003</v>
@@ -10301,7 +10364,7 @@
         <v>111</v>
       </c>
       <c r="B147" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C147" s="86">
         <v>31.395</v>
@@ -10321,7 +10384,7 @@
         <v>29</v>
       </c>
       <c r="B148" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C148" s="86">
         <v>31.884</v>
@@ -10365,7 +10428,7 @@
         <v>30</v>
       </c>
       <c r="B149" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C149" s="86">
         <v>46.018000000000001</v>
@@ -10409,7 +10472,7 @@
         <v>31</v>
       </c>
       <c r="B150" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C150" s="86">
         <v>44.023000000000003</v>
@@ -10453,7 +10516,7 @@
         <v>37</v>
       </c>
       <c r="B151" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C151" s="86">
         <v>35.158999999999999</v>
@@ -10497,7 +10560,7 @@
         <v>38</v>
       </c>
       <c r="B152" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C152" s="86">
         <v>35.792000000000002</v>
@@ -10538,7 +10601,7 @@
     </row>
     <row r="153" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A153" s="76" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C153" s="78"/>
       <c r="D153" s="75"/>
@@ -10564,7 +10627,7 @@
         <v>110</v>
       </c>
       <c r="B154" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C154" s="86">
         <v>29.59</v>
@@ -10596,7 +10659,7 @@
         <v>5</v>
       </c>
       <c r="B155" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C155" s="86">
         <v>25.742999999999999</v>
@@ -10628,7 +10691,7 @@
         <v>6</v>
       </c>
       <c r="B156" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C156" s="86">
         <v>31.568000000000001</v>
@@ -10660,7 +10723,7 @@
         <v>4</v>
       </c>
       <c r="B157" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C157" s="86">
         <v>29.98</v>
@@ -10692,7 +10755,7 @@
         <v>14</v>
       </c>
       <c r="B158" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C158" s="86">
         <v>30.077999999999999</v>
@@ -10724,7 +10787,7 @@
         <v>7</v>
       </c>
       <c r="B159" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C159" s="86">
         <v>42.079000000000001</v>
@@ -10756,7 +10819,7 @@
         <v>10</v>
       </c>
       <c r="B160" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C160" s="86">
         <v>40.741</v>
@@ -10823,7 +10886,7 @@
         <v>29</v>
       </c>
       <c r="B168" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C168" s="86">
         <v>30.861000000000001</v>
@@ -10855,7 +10918,7 @@
         <v>30</v>
       </c>
       <c r="B169" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C169" s="86">
         <v>40.048999999999999</v>
@@ -10887,7 +10950,7 @@
         <v>31</v>
       </c>
       <c r="B170" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C170" s="86">
         <v>40.097000000000001</v>
@@ -10931,7 +10994,7 @@
         <v>37</v>
       </c>
       <c r="B171" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C171" s="86">
         <v>29.138000000000002</v>
@@ -10963,7 +11026,7 @@
         <v>38</v>
       </c>
       <c r="B172" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C172" s="86">
         <v>26.065999999999999</v>
@@ -10992,7 +11055,7 @@
     </row>
     <row r="173" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A173" s="76" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C173" s="78"/>
       <c r="D173" s="75"/>
@@ -11018,7 +11081,7 @@
         <v>110</v>
       </c>
       <c r="B174" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C174" s="86">
         <v>30.728999999999999</v>
@@ -11062,7 +11125,7 @@
         <v>5</v>
       </c>
       <c r="B175" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C175" s="86">
         <v>27.041</v>
@@ -11094,7 +11157,7 @@
         <v>6</v>
       </c>
       <c r="B176" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C176" s="86">
         <v>30.611999999999998</v>
@@ -11138,7 +11201,7 @@
         <v>4</v>
       </c>
       <c r="B177" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C177" s="86">
         <v>31.632999999999999</v>
@@ -11182,7 +11245,7 @@
         <v>14</v>
       </c>
       <c r="B178" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C178" s="86">
         <v>24.242000000000001</v>
@@ -11202,7 +11265,7 @@
         <v>7</v>
       </c>
       <c r="B179" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C179" s="86">
         <v>34.831000000000003</v>
@@ -11234,7 +11297,7 @@
         <v>10</v>
       </c>
       <c r="B180" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C180" s="86">
         <v>36.517000000000003</v>
@@ -11281,7 +11344,7 @@
         <v>21</v>
       </c>
       <c r="B184" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C184" s="86">
         <v>26.486000000000001</v>
@@ -11301,7 +11364,7 @@
         <v>23</v>
       </c>
       <c r="B185" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C185" s="86">
         <v>21.622</v>
@@ -11331,7 +11394,7 @@
         <v>29</v>
       </c>
       <c r="B188" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C188" s="86">
         <v>35.106000000000002</v>
@@ -11363,7 +11426,7 @@
         <v>30</v>
       </c>
       <c r="B189" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C189" s="86">
         <v>42.697000000000003</v>
@@ -11395,7 +11458,7 @@
         <v>31</v>
       </c>
       <c r="B190" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C190" s="86">
         <v>28.414999999999999</v>
@@ -11415,7 +11478,7 @@
         <v>37</v>
       </c>
       <c r="B191" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C191" s="86">
         <v>28.646000000000001</v>
@@ -11435,7 +11498,7 @@
         <v>38</v>
       </c>
       <c r="B192" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C192" s="86">
         <v>40.984000000000002</v>
@@ -11476,7 +11539,7 @@
     </row>
     <row r="193" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A193" s="76" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C193" s="78"/>
       <c r="D193" s="75"/>
@@ -11502,7 +11565,7 @@
         <v>110</v>
       </c>
       <c r="B194" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C194" s="86">
         <v>53.933</v>
@@ -11534,7 +11597,7 @@
         <v>5</v>
       </c>
       <c r="B195" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C195" s="86">
         <v>42.164999999999999</v>
@@ -11566,7 +11629,7 @@
         <v>6</v>
       </c>
       <c r="B196" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C196" s="86">
         <v>44.384</v>
@@ -11598,7 +11661,7 @@
         <v>4</v>
       </c>
       <c r="B197" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C197" s="86">
         <v>36.212000000000003</v>
@@ -11660,7 +11723,7 @@
         <v>21</v>
       </c>
       <c r="B204" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C204" s="86">
         <v>21.013000000000002</v>
@@ -11680,7 +11743,7 @@
         <v>23</v>
       </c>
       <c r="B205" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C205" s="86">
         <v>25.312000000000001</v>
@@ -11732,7 +11795,7 @@
         <v>31</v>
       </c>
       <c r="B210" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C210" s="86">
         <v>22.535</v>
@@ -11759,7 +11822,7 @@
     </row>
     <row r="213" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A213" s="76" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C213" s="78"/>
       <c r="D213" s="75"/>
@@ -11785,7 +11848,7 @@
         <v>110</v>
       </c>
       <c r="B214" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C214" s="86">
         <v>48.289000000000001</v>
@@ -11817,7 +11880,7 @@
         <v>5</v>
       </c>
       <c r="B215" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C215" s="86">
         <v>30.038</v>
@@ -11849,7 +11912,7 @@
         <v>6</v>
       </c>
       <c r="B216" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C216" s="86">
         <v>35.938000000000002</v>
@@ -11881,7 +11944,7 @@
         <v>4</v>
       </c>
       <c r="B217" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C217" s="86">
         <v>23.077000000000002</v>
@@ -11901,7 +11964,7 @@
         <v>14</v>
       </c>
       <c r="B218" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C218" s="86">
         <v>27.099</v>
@@ -12000,7 +12063,7 @@
     </row>
     <row r="233" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A233" s="76" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C233" s="78"/>
       <c r="D233" s="75"/>
@@ -12026,7 +12089,7 @@
         <v>110</v>
       </c>
       <c r="B234" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C234" s="86">
         <v>42.856999999999999</v>
@@ -12058,7 +12121,7 @@
         <v>5</v>
       </c>
       <c r="B235" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C235" s="86">
         <v>29.63</v>
@@ -12078,7 +12141,7 @@
         <v>6</v>
       </c>
       <c r="B236" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C236" s="86">
         <v>31.788</v>
@@ -12098,7 +12161,7 @@
         <v>4</v>
       </c>
       <c r="B237" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C237" s="86">
         <v>33.332999999999998</v>
@@ -12190,7 +12253,7 @@
     </row>
     <row r="253" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A253" s="76" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C253" s="78"/>
       <c r="D253" s="75"/>
@@ -12216,7 +12279,7 @@
         <v>110</v>
       </c>
       <c r="B254" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C254" s="86">
         <v>65.191999999999993</v>
@@ -12248,7 +12311,7 @@
         <v>5</v>
       </c>
       <c r="B255" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C255" s="86">
         <v>35.064999999999998</v>
@@ -12280,7 +12343,7 @@
         <v>6</v>
       </c>
       <c r="B256" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C256" s="86">
         <v>28.428000000000001</v>
@@ -12312,7 +12375,7 @@
         <v>4</v>
       </c>
       <c r="B257" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C257" s="86">
         <v>29.878</v>
@@ -12404,7 +12467,7 @@
     </row>
     <row r="273" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A273" s="76" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C273" s="78"/>
       <c r="D273" s="75"/>
@@ -12430,7 +12493,7 @@
         <v>110</v>
       </c>
       <c r="B274" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C274" s="86">
         <v>55.161000000000001</v>
@@ -12462,7 +12525,7 @@
         <v>5</v>
       </c>
       <c r="B275" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C275" s="86">
         <v>30.547999999999998</v>
@@ -12494,7 +12557,7 @@
         <v>6</v>
       </c>
       <c r="B276" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C276" s="86">
         <v>31.138000000000002</v>
@@ -12514,7 +12577,7 @@
         <v>4</v>
       </c>
       <c r="B277" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C277" s="86">
         <v>36.024999999999999</v>
@@ -12618,7 +12681,7 @@
     </row>
     <row r="293" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A293" s="76" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C293" s="78"/>
       <c r="D293" s="75"/>
@@ -12644,7 +12707,7 @@
         <v>110</v>
       </c>
       <c r="B294" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C294" s="86">
         <v>49.057000000000002</v>
@@ -12676,7 +12739,7 @@
         <v>5</v>
       </c>
       <c r="B295" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C295" s="86">
         <v>41.698</v>
@@ -12708,7 +12771,7 @@
         <v>6</v>
       </c>
       <c r="B296" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C296" s="86">
         <v>43.023000000000003</v>
@@ -12740,7 +12803,7 @@
         <v>4</v>
       </c>
       <c r="B297" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C297" s="86">
         <v>45.942</v>
@@ -12797,7 +12860,7 @@
         <v>20</v>
       </c>
       <c r="B303" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C303" s="86">
         <v>33.39</v>
@@ -12844,7 +12907,7 @@
         <v>111</v>
       </c>
       <c r="B307" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C307" s="86">
         <v>35.104999999999997</v>
@@ -12876,7 +12939,7 @@
         <v>29</v>
       </c>
       <c r="B308" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C308" s="86">
         <v>32.223999999999997</v>
@@ -12918,7 +12981,7 @@
         <v>37</v>
       </c>
       <c r="B311" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C311" s="86">
         <v>33.834000000000003</v>
@@ -12952,7 +13015,7 @@
     </row>
     <row r="313" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A313" s="76" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C313" s="78"/>
       <c r="D313" s="75"/>
@@ -12978,7 +13041,7 @@
         <v>110</v>
       </c>
       <c r="B314" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C314" s="86">
         <v>62.131999999999998</v>
@@ -13010,7 +13073,7 @@
         <v>5</v>
       </c>
       <c r="B315" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C315" s="86">
         <v>21.454999999999998</v>
@@ -13030,7 +13093,7 @@
         <v>6</v>
       </c>
       <c r="B316" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C316" s="86">
         <v>22.321000000000002</v>
@@ -13050,7 +13113,7 @@
         <v>4</v>
       </c>
       <c r="B317" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C317" s="86">
         <v>20.312000000000001</v>
@@ -13142,7 +13205,7 @@
     </row>
     <row r="333" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A333" s="76" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C333" s="78"/>
       <c r="D333" s="75"/>
@@ -13168,7 +13231,7 @@
         <v>110</v>
       </c>
       <c r="B334" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C334" s="86">
         <v>24.155000000000001</v>
@@ -13200,7 +13263,7 @@
         <v>5</v>
       </c>
       <c r="B335" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C335" s="86">
         <v>20</v>
@@ -13220,7 +13283,7 @@
         <v>6</v>
       </c>
       <c r="B336" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C336" s="86">
         <v>15.663</v>
@@ -13240,7 +13303,7 @@
         <v>4</v>
       </c>
       <c r="B337" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C337" s="86">
         <v>19.396999999999998</v>
@@ -13272,7 +13335,7 @@
         <v>14</v>
       </c>
       <c r="B338" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C338" s="86">
         <v>38.960999999999999</v>
@@ -13309,7 +13372,7 @@
         <v>10</v>
       </c>
       <c r="B340" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C340" s="86">
         <v>47.161999999999999</v>
@@ -13371,7 +13434,7 @@
         <v>111</v>
       </c>
       <c r="B347" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C347" s="86">
         <v>33.472999999999999</v>
@@ -13403,7 +13466,7 @@
         <v>29</v>
       </c>
       <c r="B348" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C348" s="86">
         <v>40.872999999999998</v>
@@ -13440,7 +13503,7 @@
         <v>31</v>
       </c>
       <c r="B350" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C350" s="86">
         <v>36.889000000000003</v>
@@ -13472,7 +13535,7 @@
         <v>37</v>
       </c>
       <c r="B351" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C351" s="86">
         <v>40.597999999999999</v>
@@ -13504,7 +13567,7 @@
         <v>38</v>
       </c>
       <c r="B352" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C352" s="86">
         <v>46.256</v>
@@ -13533,7 +13596,7 @@
     </row>
     <row r="353" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A353" s="76" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C353" s="78"/>
       <c r="D353" s="75"/>
@@ -13559,7 +13622,7 @@
         <v>110</v>
       </c>
       <c r="B354" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C354" s="86">
         <v>57.905999999999999</v>
@@ -13591,7 +13654,7 @@
         <v>5</v>
       </c>
       <c r="B355" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C355" s="86">
         <v>44.715000000000003</v>
@@ -13623,7 +13686,7 @@
         <v>6</v>
       </c>
       <c r="B356" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C356" s="86">
         <v>51.433999999999997</v>
@@ -13655,7 +13718,7 @@
         <v>4</v>
       </c>
       <c r="B357" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C357" s="86">
         <v>53.066000000000003</v>
@@ -13759,7 +13822,7 @@
     </row>
     <row r="373" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A373" s="76" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C373" s="78"/>
       <c r="D373" s="75"/>
@@ -13805,7 +13868,7 @@
         <v>14</v>
       </c>
       <c r="B378" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C378" s="86">
         <v>28.177</v>
@@ -13825,7 +13888,7 @@
         <v>7</v>
       </c>
       <c r="B379" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C379" s="86">
         <v>48.148000000000003</v>
@@ -13845,7 +13908,7 @@
         <v>10</v>
       </c>
       <c r="B380" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C380" s="86">
         <v>45.744999999999997</v>
@@ -13875,7 +13938,7 @@
         <v>20</v>
       </c>
       <c r="B383" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C383" s="86">
         <v>38.659999999999997</v>
@@ -13920,7 +13983,7 @@
         <v>30</v>
       </c>
       <c r="B389" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C389" s="86">
         <v>34.518000000000001</v>
@@ -13940,7 +14003,7 @@
         <v>31</v>
       </c>
       <c r="B390" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C390" s="86">
         <v>27.933</v>
@@ -13965,7 +14028,7 @@
         <v>38</v>
       </c>
       <c r="B392" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C392" s="86">
         <v>26.065999999999999</v>
@@ -13994,7 +14057,7 @@
     </row>
     <row r="393" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A393" s="76" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C393" s="78"/>
       <c r="D393" s="75"/>
@@ -14040,7 +14103,7 @@
         <v>14</v>
       </c>
       <c r="B398" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C398" s="86">
         <v>35.735999999999997</v>
@@ -14060,7 +14123,7 @@
         <v>7</v>
       </c>
       <c r="B399" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C399" s="86">
         <v>42.759</v>
@@ -14080,7 +14143,7 @@
         <v>10</v>
       </c>
       <c r="B400" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C400" s="86">
         <v>41.801000000000002</v>
@@ -14100,7 +14163,7 @@
         <v>17</v>
       </c>
       <c r="B401" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C401" s="86">
         <v>27.419</v>
@@ -14125,7 +14188,7 @@
         <v>20</v>
       </c>
       <c r="B403" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C403" s="86">
         <v>41.801000000000002</v>
@@ -14157,7 +14220,7 @@
         <v>21</v>
       </c>
       <c r="B404" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C404" s="86">
         <v>27.66</v>
@@ -14177,7 +14240,7 @@
         <v>23</v>
       </c>
       <c r="B405" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C405" s="86">
         <v>28.664000000000001</v>
@@ -14202,7 +14265,7 @@
         <v>111</v>
       </c>
       <c r="B407" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C407" s="86">
         <v>30.853999999999999</v>
@@ -14234,7 +14297,7 @@
         <v>29</v>
       </c>
       <c r="B408" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C408" s="86">
         <v>20.925000000000001</v>
@@ -14266,7 +14329,7 @@
         <v>30</v>
       </c>
       <c r="B409" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C409" s="86">
         <v>37.729999999999997</v>
@@ -14298,7 +14361,7 @@
         <v>31</v>
       </c>
       <c r="B410" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C410" s="86">
         <v>41.103999999999999</v>
@@ -14318,7 +14381,7 @@
         <v>37</v>
       </c>
       <c r="B411" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C411" s="86">
         <v>30.768999999999998</v>
@@ -14350,7 +14413,7 @@
         <v>38</v>
       </c>
       <c r="B412" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C412" s="86">
         <v>29.282</v>
@@ -14379,7 +14442,7 @@
     </row>
     <row r="413" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A413" s="76" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C413" s="78"/>
       <c r="D413" s="75"/>
@@ -14425,7 +14488,7 @@
         <v>14</v>
       </c>
       <c r="B418" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C418" s="86">
         <v>20.472000000000001</v>
@@ -14445,7 +14508,7 @@
         <v>7</v>
       </c>
       <c r="B419" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C419" s="86">
         <v>50.41</v>
@@ -14477,7 +14540,7 @@
         <v>10</v>
       </c>
       <c r="B420" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C420" s="86">
         <v>52.652999999999999</v>
@@ -14509,7 +14572,7 @@
         <v>17</v>
       </c>
       <c r="B421" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C421" s="86">
         <v>28.193999999999999</v>
@@ -14541,7 +14604,7 @@
         <v>19</v>
       </c>
       <c r="B422" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C422" s="86">
         <v>34.978999999999999</v>
@@ -14573,7 +14636,7 @@
         <v>20</v>
       </c>
       <c r="B423" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C423" s="86">
         <v>50.204000000000001</v>
@@ -14605,7 +14668,7 @@
         <v>21</v>
       </c>
       <c r="B424" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C424" s="86">
         <v>29.957999999999998</v>
@@ -14640,7 +14703,7 @@
         <v>29</v>
       </c>
       <c r="B428" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C428" s="86">
         <v>22.917000000000002</v>
@@ -14660,7 +14723,7 @@
         <v>30</v>
       </c>
       <c r="B429" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C429" s="86">
         <v>24.893000000000001</v>
@@ -14680,7 +14743,7 @@
         <v>31</v>
       </c>
       <c r="B430" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C430" s="86">
         <v>25.640999999999998</v>
@@ -14700,7 +14763,7 @@
         <v>37</v>
       </c>
       <c r="B431" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C431" s="86">
         <v>23.707000000000001</v>
@@ -14720,7 +14783,7 @@
         <v>38</v>
       </c>
       <c r="B432" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C432" s="86">
         <v>39.326000000000001</v>
@@ -14749,7 +14812,7 @@
     </row>
     <row r="433" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A433" s="76" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C433" s="78"/>
       <c r="D433" s="75"/>
@@ -14795,7 +14858,7 @@
         <v>14</v>
       </c>
       <c r="B438" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C438" s="86">
         <v>37.319000000000003</v>
@@ -14827,7 +14890,7 @@
         <v>7</v>
       </c>
       <c r="B439" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C439" s="86">
         <v>56.87</v>
@@ -14859,7 +14922,7 @@
         <v>10</v>
       </c>
       <c r="B440" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C440" s="86">
         <v>67.578000000000003</v>
@@ -14921,7 +14984,7 @@
         <v>111</v>
       </c>
       <c r="B447" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C447" s="86">
         <v>31.033999999999999</v>
@@ -14973,7 +15036,7 @@
         <v>38</v>
       </c>
       <c r="B452" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C452" s="86">
         <v>31.988</v>
@@ -15002,7 +15065,7 @@
     </row>
     <row r="453" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A453" s="76" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C453" s="78"/>
       <c r="D453" s="75"/>
@@ -15053,7 +15116,7 @@
         <v>7</v>
       </c>
       <c r="B459" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C459" s="86">
         <v>51.079000000000001</v>
@@ -15085,7 +15148,7 @@
         <v>10</v>
       </c>
       <c r="B460" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C460" s="86">
         <v>51.087000000000003</v>
@@ -15117,7 +15180,7 @@
         <v>17</v>
       </c>
       <c r="B461" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C461" s="86">
         <v>34.615000000000002</v>
@@ -15137,7 +15200,7 @@
         <v>19</v>
       </c>
       <c r="B462" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C462" s="86">
         <v>46.61</v>
@@ -15169,7 +15232,7 @@
         <v>20</v>
       </c>
       <c r="B463" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C463" s="86">
         <v>49.6</v>
@@ -15241,7 +15304,7 @@
         <v>38</v>
       </c>
       <c r="B472" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C472" s="86">
         <v>41.875</v>
@@ -15270,7 +15333,7 @@
     </row>
     <row r="473" spans="1:20" s="77" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A473" s="76" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C473" s="78"/>
       <c r="D473" s="75"/>
@@ -15316,7 +15379,7 @@
         <v>14</v>
       </c>
       <c r="B478" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C478" s="86">
         <v>33.43</v>
@@ -15348,7 +15411,7 @@
         <v>7</v>
       </c>
       <c r="B479" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C479" s="86">
         <v>59.433999999999997</v>
@@ -15380,7 +15443,7 @@
         <v>10</v>
       </c>
       <c r="B480" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C480" s="86">
         <v>62.286999999999999</v>
@@ -15452,7 +15515,7 @@
         <v>30</v>
       </c>
       <c r="B489" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C489" s="86">
         <v>55.610999999999997</v>
@@ -15484,7 +15547,7 @@
         <v>31</v>
       </c>
       <c r="B490" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C490" s="86">
         <v>57.613999999999997</v>
@@ -15521,7 +15584,7 @@
         <v>38</v>
       </c>
       <c r="B492" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C492" s="86">
         <v>39.003</v>

</xml_diff>